<commit_message>
Update control de tareas
</commit_message>
<xml_diff>
--- a/Otros/SCM.xlsx
+++ b/Otros/SCM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\UVG\5to Semestre\Algoritmos y Estructuras de Datos\Proyecto01-Fase-2\Otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B3FEFB-76CB-448F-A06E-9AB13F0003AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7C2CE1-6543-441A-9293-0F39B44C7F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{CBED493F-EADE-4015-8AC5-39EFF1A52CFB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Tarea</t>
   </si>
@@ -193,13 +193,19 @@
   </si>
   <si>
     <t>PDF entrega</t>
+  </si>
+  <si>
+    <t>ceafcf103efdaa8abebfd7d33e771cbaf3007b83</t>
+  </si>
+  <si>
+    <t>Programa completo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +225,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +253,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -283,18 +313,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -302,13 +339,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21741BB-77D7-4741-A085-587B0F9F358D}">
   <dimension ref="A2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="71" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:D25"/>
+    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,462 +685,422 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="H4" s="2" t="s">
+      <c r="F4" s="2"/>
+      <c r="H4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="H6" s="1" t="s">
+      <c r="F6" s="2"/>
+      <c r="H6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="H7" s="1" t="s">
+      <c r="F7" s="2"/>
+      <c r="H7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="H8" s="1" t="s">
+      <c r="F8" s="2"/>
+      <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="H9" s="1" t="s">
+      <c r="F9" s="2"/>
+      <c r="H9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="H10" s="1" t="s">
+      <c r="F10" s="2"/>
+      <c r="H10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="H11" s="1" t="s">
+      <c r="F11" s="2"/>
+      <c r="H11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="H12" s="1" t="s">
+      <c r="F12" s="2"/>
+      <c r="H12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="2"/>
+      <c r="H13" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C2:D3"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E5:F5"/>
@@ -1106,20 +1117,65 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>